<commit_message>
Updated Project added 3 more column - worked Hours, vacation & bank holiday
</commit_message>
<xml_diff>
--- a/assets/full_pay.xlsx
+++ b/assets/full_pay.xlsx
@@ -2,27 +2,43 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="930" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
+      <charset val="1"/>
       <family val="2"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="3">
@@ -35,7 +51,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -48,17 +64,41 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="6">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="5">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" name="Comma" xfId="1"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
+    <cellStyle builtinId="4" name="Currency" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="5" name="Percent" xfId="5"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -141,44 +181,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -205,15 +245,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -240,7 +279,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -252,231 +290,274 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L178"/>
+  <dimension ref="A1:O178"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" xSplit="0" ySplit="1"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="M5" activeCellId="0" pane="bottomLeft" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.58203125" defaultRowHeight="13.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col width="7.5703125" customWidth="1" min="1" max="1"/>
-    <col width="7.140625" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="21.7109375" customWidth="1" min="3" max="3"/>
-    <col width="28.85546875" customWidth="1" min="4" max="4"/>
-    <col width="19.5703125" customWidth="1" min="5" max="5"/>
-    <col width="17.140625" customWidth="1" min="6" max="6"/>
-    <col width="8" customWidth="1" min="7" max="7"/>
-    <col width="10.140625" bestFit="1" customWidth="1" min="8" max="8"/>
-    <col width="8.7109375" customWidth="1" min="9" max="9"/>
-    <col width="8.7109375" bestFit="1" customWidth="1" min="10" max="10"/>
-    <col width="12.85546875" bestFit="1" customWidth="1" min="11" max="11"/>
-    <col width="11.7109375" customWidth="1" min="12" max="12"/>
+    <col customWidth="1" max="1" min="1" style="3" width="7.57"/>
+    <col customWidth="1" max="2" min="2" style="3" width="7.14"/>
+    <col customWidth="1" max="3" min="3" style="3" width="21.72"/>
+    <col customWidth="1" max="4" min="4" style="3" width="28.86"/>
+    <col customWidth="1" max="5" min="5" style="3" width="19.57"/>
+    <col customWidth="1" max="6" min="6" style="3" width="17.14"/>
+    <col customWidth="1" max="7" min="7" style="3" width="8"/>
+    <col customWidth="1" max="8" min="8" style="3" width="10.14"/>
+    <col customWidth="1" max="10" min="9" style="3" width="8.710000000000001"/>
+    <col customWidth="1" max="11" min="11" style="3" width="12.86"/>
+    <col customWidth="1" max="12" min="12" style="3" width="10.18"/>
+    <col customWidth="1" max="13" min="13" style="3" width="10.55"/>
+    <col customWidth="1" max="14" min="14" style="3" width="12.26"/>
+    <col customWidth="1" max="15" min="15" style="3" width="11.71"/>
+    <col customWidth="1" max="1024" min="1024" style="3" width="10.17"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row customFormat="1" customHeight="1" ht="13.8" r="1" s="4">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>period</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>emp nr</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>em name</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>address</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>city</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>niss nr</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>price hr</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>hr contract</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>meal voucher</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>chomage</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" s="4" t="inlineStr">
         <is>
           <t>worked hours</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" s="4" t="inlineStr">
+        <is>
+          <t>no_work</t>
+        </is>
+      </c>
+      <c r="M1" s="4" t="inlineStr">
+        <is>
+          <t>vacation</t>
+        </is>
+      </c>
+      <c r="N1" s="4" t="inlineStr">
+        <is>
+          <t>bank_holiday</t>
+        </is>
+      </c>
+      <c r="O1" s="4" t="inlineStr">
         <is>
           <t>netto</t>
         </is>
@@ -536,6 +617,17 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
           <t>1.093,05</t>
         </is>
       </c>
@@ -592,7 +684,14 @@
           <t>66</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
         <is>
           <t>1.341,73</t>
         </is>
@@ -652,6 +751,17 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
+          <t>6:00</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
           <t>1.495,05</t>
         </is>
       </c>
@@ -708,7 +818,14 @@
           <t>52</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
         <is>
           <t>697,86</t>
         </is>
@@ -758,7 +875,10 @@
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr">
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr">
         <is>
           <t>0,00</t>
         </is>
@@ -816,7 +936,14 @@
           <t>139</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
         <is>
           <t>1.701,54</t>
         </is>
@@ -876,6 +1003,17 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
+          <t>62:00</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
           <t>693,90</t>
         </is>
       </c>
@@ -934,6 +1072,17 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
+          <t>40:00</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
           <t>1.402,59</t>
         </is>
       </c>
@@ -991,6 +1140,17 @@
         </is>
       </c>
       <c r="L10" t="inlineStr">
+        <is>
+          <t>78:00</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>6:00</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
         <is>
           <t>570,76</t>
         </is>
@@ -1040,7 +1200,10 @@
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr">
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr">
         <is>
           <t>0,00</t>
         </is>
@@ -1090,7 +1253,10 @@
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr">
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr">
         <is>
           <t>0,00</t>
         </is>
@@ -1148,7 +1314,18 @@
           <t>92</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr">
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
         <is>
           <t>1.247,94</t>
         </is>
@@ -1206,7 +1383,14 @@
           <t>115</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
         <is>
           <t>1.276,96</t>
         </is>
@@ -1266,6 +1450,21 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
+          <t>31:00</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
           <t>1.265,22</t>
         </is>
       </c>
@@ -1322,7 +1521,14 @@
           <t>145</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr">
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
         <is>
           <t>1.694,07</t>
         </is>
@@ -1381,6 +1587,17 @@
         </is>
       </c>
       <c r="L17" t="inlineStr">
+        <is>
+          <t>24:00</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>9:00</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
         <is>
           <t>1.155,80</t>
         </is>
@@ -1432,6 +1649,13 @@
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr">
         <is>
+          <t>45:00</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr">
+        <is>
           <t>0,00</t>
         </is>
       </c>
@@ -1489,6 +1713,21 @@
         </is>
       </c>
       <c r="L19" t="inlineStr">
+        <is>
+          <t>44:00</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
         <is>
           <t>659,28</t>
         </is>
@@ -1538,7 +1777,10 @@
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr">
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr">
         <is>
           <t>0,00</t>
         </is>
@@ -1588,7 +1830,14 @@
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr">
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
         <is>
           <t>1.157,69</t>
         </is>
@@ -1648,6 +1897,21 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
+          <t>7:00</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>7:00</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
           <t>1.247,63</t>
         </is>
       </c>
@@ -1706,6 +1970,17 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
+          <t>62:00</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
           <t>277,88</t>
         </is>
       </c>
@@ -1764,6 +2039,21 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>7:00</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>6:00</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
           <t>911,08</t>
         </is>
       </c>
@@ -1822,6 +2112,17 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
           <t>1.525,33</t>
         </is>
       </c>
@@ -1878,7 +2179,18 @@
           <t>93</t>
         </is>
       </c>
-      <c r="L26" t="inlineStr">
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
         <is>
           <t>1.288,65</t>
         </is>
@@ -1938,6 +2250,21 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
+          <t>7:00</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
           <t>1.251,74</t>
         </is>
       </c>
@@ -1994,7 +2321,18 @@
           <t>127</t>
         </is>
       </c>
-      <c r="L28" t="inlineStr">
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
         <is>
           <t>1.597,02</t>
         </is>
@@ -2054,6 +2392,17 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
+          <t>36:00</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
           <t>1.258,90</t>
         </is>
       </c>
@@ -2110,7 +2459,14 @@
           <t>77</t>
         </is>
       </c>
-      <c r="L30" t="inlineStr">
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
         <is>
           <t>1.640,10</t>
         </is>
@@ -2168,7 +2524,14 @@
           <t>115</t>
         </is>
       </c>
-      <c r="L31" t="inlineStr">
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>7:00</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
         <is>
           <t>1.598,42</t>
         </is>
@@ -2226,7 +2589,14 @@
           <t>56</t>
         </is>
       </c>
-      <c r="L32" t="inlineStr">
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
         <is>
           <t>1.443,45</t>
         </is>
@@ -2285,6 +2655,17 @@
         </is>
       </c>
       <c r="L33" t="inlineStr">
+        <is>
+          <t>51:00</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr"/>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
         <is>
           <t>1.265,22</t>
         </is>
@@ -2334,7 +2715,10 @@
       <c r="I34" t="inlineStr"/>
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr"/>
-      <c r="L34" t="inlineStr">
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr"/>
+      <c r="N34" t="inlineStr"/>
+      <c r="O34" t="inlineStr">
         <is>
           <t>0,00</t>
         </is>
@@ -2394,6 +2778,21 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>39:00</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>6:00</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
           <t>800,08</t>
         </is>
       </c>
@@ -2450,7 +2849,18 @@
           <t>120</t>
         </is>
       </c>
-      <c r="L36" t="inlineStr">
+      <c r="L36" t="inlineStr"/>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
         <is>
           <t>1.527,56</t>
         </is>
@@ -2508,7 +2918,18 @@
           <t>115</t>
         </is>
       </c>
-      <c r="L37" t="inlineStr">
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>30:00</t>
+        </is>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
         <is>
           <t>1.464,57</t>
         </is>
@@ -2566,7 +2987,18 @@
           <t>104</t>
         </is>
       </c>
-      <c r="L38" t="inlineStr">
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>44:00</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
         <is>
           <t>1.407,98</t>
         </is>
@@ -2626,6 +3058,17 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
+          <t>60:00</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr"/>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>6:00</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
           <t>716,15</t>
         </is>
       </c>
@@ -2684,6 +3127,17 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr"/>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
           <t>1.385,61</t>
         </is>
       </c>
@@ -2740,7 +3194,14 @@
           <t>98</t>
         </is>
       </c>
-      <c r="L41" t="inlineStr">
+      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr"/>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>7:00</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
         <is>
           <t>1.247,19</t>
         </is>
@@ -2800,6 +3261,21 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
+          <t>22:00</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>32:00</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
           <t>1.128,89</t>
         </is>
       </c>
@@ -2856,7 +3332,18 @@
           <t>46</t>
         </is>
       </c>
-      <c r="L43" t="inlineStr">
+      <c r="L43" t="inlineStr"/>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>98:00</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
         <is>
           <t>712,80</t>
         </is>
@@ -2914,7 +3401,14 @@
           <t>150</t>
         </is>
       </c>
-      <c r="L44" t="inlineStr">
+      <c r="L44" t="inlineStr"/>
+      <c r="M44" t="inlineStr"/>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>7:00</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
         <is>
           <t>1.667,16</t>
         </is>
@@ -2974,6 +3468,21 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>9:00</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
           <t>1.022,85</t>
         </is>
       </c>
@@ -3030,7 +3539,14 @@
           <t>148</t>
         </is>
       </c>
-      <c r="L46" t="inlineStr">
+      <c r="L46" t="inlineStr"/>
+      <c r="M46" t="inlineStr"/>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
         <is>
           <t>1.627,28</t>
         </is>
@@ -3090,6 +3606,17 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr"/>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
           <t>1.551,62</t>
         </is>
       </c>
@@ -3148,6 +3675,17 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr"/>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>9:00</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
           <t>1.567,25</t>
         </is>
       </c>
@@ -3206,6 +3744,17 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
+          <t>6:00</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr"/>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
           <t>1.391,16</t>
         </is>
       </c>
@@ -3264,6 +3813,17 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
+          <t>9:00</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr"/>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>5:00</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
           <t>1.496,83</t>
         </is>
       </c>
@@ -3320,7 +3880,14 @@
           <t>141</t>
         </is>
       </c>
-      <c r="L51" t="inlineStr">
+      <c r="L51" t="inlineStr"/>
+      <c r="M51" t="inlineStr"/>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="O51" t="inlineStr">
         <is>
           <t>1.713,90</t>
         </is>
@@ -3380,6 +3947,21 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
           <t>1.318,47</t>
         </is>
       </c>
@@ -3436,7 +4018,14 @@
           <t>114</t>
         </is>
       </c>
-      <c r="L53" t="inlineStr">
+      <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr">
         <is>
           <t>1.682,77</t>
         </is>
@@ -3486,7 +4075,10 @@
       <c r="I54" t="inlineStr"/>
       <c r="J54" t="inlineStr"/>
       <c r="K54" t="inlineStr"/>
-      <c r="L54" t="inlineStr">
+      <c r="L54" t="inlineStr"/>
+      <c r="M54" t="inlineStr"/>
+      <c r="N54" t="inlineStr"/>
+      <c r="O54" t="inlineStr">
         <is>
           <t>0,00</t>
         </is>
@@ -3546,6 +4138,17 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
+          <t>40:00</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr"/>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>6:00</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
           <t>880,71</t>
         </is>
       </c>
@@ -3604,6 +4207,17 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
+          <t>73:00</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr"/>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>5:00</t>
+        </is>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
           <t>429,09</t>
         </is>
       </c>
@@ -3660,7 +4274,14 @@
           <t>102</t>
         </is>
       </c>
-      <c r="L57" t="inlineStr">
+      <c r="L57" t="inlineStr"/>
+      <c r="M57" t="inlineStr"/>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="O57" t="inlineStr">
         <is>
           <t>1.419,86</t>
         </is>
@@ -3720,6 +4341,17 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
+          <t>39:00</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr"/>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>3:00</t>
+        </is>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
           <t>462,86</t>
         </is>
       </c>
@@ -3777,6 +4409,17 @@
         </is>
       </c>
       <c r="L59" t="inlineStr">
+        <is>
+          <t>72:00</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr"/>
+      <c r="N59" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="O59" t="inlineStr">
         <is>
           <t>911,17</t>
         </is>
@@ -3830,7 +4473,18 @@
           <t>7</t>
         </is>
       </c>
-      <c r="L60" t="inlineStr">
+      <c r="L60" t="inlineStr"/>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>145:00</t>
+        </is>
+      </c>
+      <c r="N60" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="O60" t="inlineStr">
         <is>
           <t>174,85</t>
         </is>
@@ -3888,7 +4542,10 @@
           <t>48</t>
         </is>
       </c>
-      <c r="L61" t="inlineStr">
+      <c r="L61" t="inlineStr"/>
+      <c r="M61" t="inlineStr"/>
+      <c r="N61" t="inlineStr"/>
+      <c r="O61" t="inlineStr">
         <is>
           <t>615,85</t>
         </is>
@@ -3938,7 +4595,14 @@
       <c r="I62" t="inlineStr"/>
       <c r="J62" t="inlineStr"/>
       <c r="K62" t="inlineStr"/>
-      <c r="L62" t="inlineStr">
+      <c r="L62" t="inlineStr"/>
+      <c r="M62" t="inlineStr"/>
+      <c r="N62" t="inlineStr">
+        <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="O62" t="inlineStr">
         <is>
           <t>1.121,34</t>
         </is>
@@ -3998,6 +4662,13 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
+          <t>30:00</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr"/>
+      <c r="N63" t="inlineStr"/>
+      <c r="O63" t="inlineStr">
+        <is>
           <t>510,30</t>
         </is>
       </c>
@@ -4056,6 +4727,17 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
+          <t>34:00</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr"/>
+      <c r="N64" t="inlineStr">
+        <is>
+          <t>7:00</t>
+        </is>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
           <t>1.323,02</t>
         </is>
       </c>
@@ -4114,6 +4796,17 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr"/>
+      <c r="N65" t="inlineStr">
+        <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
           <t>1.285,85</t>
         </is>
       </c>
@@ -4172,6 +4865,17 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="M66" t="inlineStr"/>
+      <c r="N66" t="inlineStr">
+        <is>
+          <t>3:00</t>
+        </is>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
           <t>675,50</t>
         </is>
       </c>
@@ -4229,6 +4933,21 @@
         </is>
       </c>
       <c r="L67" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="N67" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="O67" t="inlineStr">
         <is>
           <t>1.593,93</t>
         </is>
@@ -4280,6 +4999,17 @@
       <c r="K68" t="inlineStr"/>
       <c r="L68" t="inlineStr">
         <is>
+          <t>154:00</t>
+        </is>
+      </c>
+      <c r="M68" t="inlineStr"/>
+      <c r="N68" t="inlineStr">
+        <is>
+          <t>6:00</t>
+        </is>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
           <t>70,06</t>
         </is>
       </c>
@@ -4338,6 +5068,17 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
+          <t>84:00</t>
+        </is>
+      </c>
+      <c r="M69" t="inlineStr"/>
+      <c r="N69" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
           <t>696,73</t>
         </is>
       </c>
@@ -4395,6 +5136,21 @@
         </is>
       </c>
       <c r="L70" t="inlineStr">
+        <is>
+          <t>22:00</t>
+        </is>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="N70" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="O70" t="inlineStr">
         <is>
           <t>1.383,96</t>
         </is>
@@ -4444,7 +5200,10 @@
       <c r="I71" t="inlineStr"/>
       <c r="J71" t="inlineStr"/>
       <c r="K71" t="inlineStr"/>
-      <c r="L71" t="inlineStr">
+      <c r="L71" t="inlineStr"/>
+      <c r="M71" t="inlineStr"/>
+      <c r="N71" t="inlineStr"/>
+      <c r="O71" t="inlineStr">
         <is>
           <t>0,00</t>
         </is>
@@ -4498,7 +5257,18 @@
           <t>131</t>
         </is>
       </c>
-      <c r="L72" t="inlineStr">
+      <c r="L72" t="inlineStr"/>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="N72" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="O72" t="inlineStr">
         <is>
           <t>1.750,81</t>
         </is>
@@ -4558,6 +5328,17 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
+          <t>32:00</t>
+        </is>
+      </c>
+      <c r="M73" t="inlineStr"/>
+      <c r="N73" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
           <t>1.419,72</t>
         </is>
       </c>
@@ -4616,6 +5397,17 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
+          <t>43:00</t>
+        </is>
+      </c>
+      <c r="M74" t="inlineStr"/>
+      <c r="N74" t="inlineStr">
+        <is>
+          <t>3:00</t>
+        </is>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
           <t>568,70</t>
         </is>
       </c>
@@ -4674,6 +5466,17 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="M75" t="inlineStr"/>
+      <c r="N75" t="inlineStr">
+        <is>
+          <t>3:00</t>
+        </is>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
           <t>479,45</t>
         </is>
       </c>
@@ -4732,6 +5535,17 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
+          <t>31:00</t>
+        </is>
+      </c>
+      <c r="M76" t="inlineStr"/>
+      <c r="N76" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
           <t>1.493,50</t>
         </is>
       </c>
@@ -4790,6 +5604,17 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
+          <t>27:00</t>
+        </is>
+      </c>
+      <c r="M77" t="inlineStr"/>
+      <c r="N77" t="inlineStr">
+        <is>
+          <t>5:00</t>
+        </is>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
           <t>1.418,52</t>
         </is>
       </c>
@@ -4847,6 +5672,21 @@
         </is>
       </c>
       <c r="L78" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>57:00</t>
+        </is>
+      </c>
+      <c r="N78" t="inlineStr">
+        <is>
+          <t>5:00</t>
+        </is>
+      </c>
+      <c r="O78" t="inlineStr">
         <is>
           <t>1.109,56</t>
         </is>
@@ -4898,6 +5738,13 @@
       <c r="K79" t="inlineStr"/>
       <c r="L79" t="inlineStr">
         <is>
+          <t>34:00</t>
+        </is>
+      </c>
+      <c r="M79" t="inlineStr"/>
+      <c r="N79" t="inlineStr"/>
+      <c r="O79" t="inlineStr">
+        <is>
           <t>0,00</t>
         </is>
       </c>
@@ -4948,6 +5795,17 @@
       <c r="K80" t="inlineStr"/>
       <c r="L80" t="inlineStr">
         <is>
+          <t>138:00</t>
+        </is>
+      </c>
+      <c r="M80" t="inlineStr"/>
+      <c r="N80" t="inlineStr">
+        <is>
+          <t>7:00</t>
+        </is>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
           <t>80,75</t>
         </is>
       </c>
@@ -5004,7 +5862,14 @@
           <t>48</t>
         </is>
       </c>
-      <c r="L81" t="inlineStr">
+      <c r="L81" t="inlineStr"/>
+      <c r="M81" t="inlineStr"/>
+      <c r="N81" t="inlineStr">
+        <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="O81" t="inlineStr">
         <is>
           <t>1.042,06</t>
         </is>
@@ -5064,6 +5929,17 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="M82" t="inlineStr"/>
+      <c r="N82" t="inlineStr">
+        <is>
+          <t>3:00</t>
+        </is>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
           <t>780,12</t>
         </is>
       </c>
@@ -5122,6 +5998,17 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
+          <t>26:00</t>
+        </is>
+      </c>
+      <c r="M83" t="inlineStr"/>
+      <c r="N83" t="inlineStr">
+        <is>
+          <t>5:00</t>
+        </is>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
           <t>1.319,51</t>
         </is>
       </c>
@@ -5180,6 +6067,17 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
+          <t>58:00</t>
+        </is>
+      </c>
+      <c r="M84" t="inlineStr"/>
+      <c r="N84" t="inlineStr">
+        <is>
+          <t>6:00</t>
+        </is>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
           <t>828,43</t>
         </is>
       </c>
@@ -5238,6 +6136,17 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
+          <t>62:00</t>
+        </is>
+      </c>
+      <c r="M85" t="inlineStr"/>
+      <c r="N85" t="inlineStr">
+        <is>
+          <t>6:00</t>
+        </is>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
           <t>847,50</t>
         </is>
       </c>
@@ -5294,7 +6203,18 @@
           <t>46</t>
         </is>
       </c>
-      <c r="L86" t="inlineStr">
+      <c r="L86" t="inlineStr"/>
+      <c r="M86" t="inlineStr">
+        <is>
+          <t>3:00</t>
+        </is>
+      </c>
+      <c r="N86" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="O86" t="inlineStr">
         <is>
           <t>656,08</t>
         </is>
@@ -5346,6 +6266,17 @@
       <c r="K87" t="inlineStr"/>
       <c r="L87" t="inlineStr">
         <is>
+          <t>154:00</t>
+        </is>
+      </c>
+      <c r="M87" t="inlineStr"/>
+      <c r="N87" t="inlineStr">
+        <is>
+          <t>6:00</t>
+        </is>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
           <t>67,64</t>
         </is>
       </c>
@@ -5402,7 +6333,14 @@
           <t>96</t>
         </is>
       </c>
-      <c r="L88" t="inlineStr">
+      <c r="L88" t="inlineStr"/>
+      <c r="M88" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="N88" t="inlineStr"/>
+      <c r="O88" t="inlineStr">
         <is>
           <t>1.124,64</t>
         </is>
@@ -5462,6 +6400,21 @@
       </c>
       <c r="L89" t="inlineStr">
         <is>
+          <t>53:00</t>
+        </is>
+      </c>
+      <c r="M89" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="N89" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
           <t>1.118,76</t>
         </is>
       </c>
@@ -5518,7 +6471,14 @@
           <t>43</t>
         </is>
       </c>
-      <c r="L90" t="inlineStr">
+      <c r="L90" t="inlineStr"/>
+      <c r="M90" t="inlineStr"/>
+      <c r="N90" t="inlineStr">
+        <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="O90" t="inlineStr">
         <is>
           <t>965,64</t>
         </is>
@@ -5578,6 +6538,17 @@
       </c>
       <c r="L91" t="inlineStr">
         <is>
+          <t>42:00</t>
+        </is>
+      </c>
+      <c r="M91" t="inlineStr"/>
+      <c r="N91" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
           <t>1.219,65</t>
         </is>
       </c>
@@ -5636,6 +6607,17 @@
       </c>
       <c r="L92" t="inlineStr">
         <is>
+          <t>82:00</t>
+        </is>
+      </c>
+      <c r="M92" t="inlineStr"/>
+      <c r="N92" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="O92" t="inlineStr">
+        <is>
           <t>888,19</t>
         </is>
       </c>
@@ -5694,6 +6676,17 @@
       </c>
       <c r="L93" t="inlineStr">
         <is>
+          <t>40:00</t>
+        </is>
+      </c>
+      <c r="M93" t="inlineStr"/>
+      <c r="N93" t="inlineStr">
+        <is>
+          <t>7:00</t>
+        </is>
+      </c>
+      <c r="O93" t="inlineStr">
+        <is>
           <t>1.018,51</t>
         </is>
       </c>
@@ -5750,7 +6743,18 @@
           <t>46</t>
         </is>
       </c>
-      <c r="L94" t="inlineStr">
+      <c r="L94" t="inlineStr"/>
+      <c r="M94" t="inlineStr">
+        <is>
+          <t>80:00</t>
+        </is>
+      </c>
+      <c r="N94" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="O94" t="inlineStr">
         <is>
           <t>680,64</t>
         </is>
@@ -5808,7 +6812,10 @@
           <t>80</t>
         </is>
       </c>
-      <c r="L95" t="inlineStr">
+      <c r="L95" t="inlineStr"/>
+      <c r="M95" t="inlineStr"/>
+      <c r="N95" t="inlineStr"/>
+      <c r="O95" t="inlineStr">
         <is>
           <t>946,54</t>
         </is>
@@ -5867,6 +6874,17 @@
         </is>
       </c>
       <c r="L96" t="inlineStr">
+        <is>
+          <t>56:00</t>
+        </is>
+      </c>
+      <c r="M96" t="inlineStr"/>
+      <c r="N96" t="inlineStr">
+        <is>
+          <t>6:00</t>
+        </is>
+      </c>
+      <c r="O96" t="inlineStr">
         <is>
           <t>790,80</t>
         </is>
@@ -5918,6 +6936,21 @@
       <c r="K97" t="inlineStr"/>
       <c r="L97" t="inlineStr">
         <is>
+          <t>64:00</t>
+        </is>
+      </c>
+      <c r="M97" t="inlineStr">
+        <is>
+          <t>78:00</t>
+        </is>
+      </c>
+      <c r="N97" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="O97" t="inlineStr">
+        <is>
           <t>158,91</t>
         </is>
       </c>
@@ -5974,7 +7007,18 @@
           <t>106</t>
         </is>
       </c>
-      <c r="L98" t="inlineStr">
+      <c r="L98" t="inlineStr"/>
+      <c r="M98" t="inlineStr">
+        <is>
+          <t>34:00</t>
+        </is>
+      </c>
+      <c r="N98" t="inlineStr">
+        <is>
+          <t>7:00</t>
+        </is>
+      </c>
+      <c r="O98" t="inlineStr">
         <is>
           <t>1.317,29</t>
         </is>
@@ -6034,6 +7078,17 @@
       </c>
       <c r="L99" t="inlineStr">
         <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="M99" t="inlineStr"/>
+      <c r="N99" t="inlineStr">
+        <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="O99" t="inlineStr">
+        <is>
           <t>544,85</t>
         </is>
       </c>
@@ -6090,7 +7145,18 @@
           <t>71</t>
         </is>
       </c>
-      <c r="L100" t="inlineStr">
+      <c r="L100" t="inlineStr"/>
+      <c r="M100" t="inlineStr">
+        <is>
+          <t>51:00</t>
+        </is>
+      </c>
+      <c r="N100" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="O100" t="inlineStr">
         <is>
           <t>885,74</t>
         </is>
@@ -6150,6 +7216,17 @@
       </c>
       <c r="L101" t="inlineStr">
         <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="M101" t="inlineStr"/>
+      <c r="N101" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="O101" t="inlineStr">
+        <is>
           <t>1.273,63</t>
         </is>
       </c>
@@ -6206,7 +7283,18 @@
           <t>140</t>
         </is>
       </c>
-      <c r="L102" t="inlineStr">
+      <c r="L102" t="inlineStr"/>
+      <c r="M102" t="inlineStr">
+        <is>
+          <t>3:00</t>
+        </is>
+      </c>
+      <c r="N102" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="O102" t="inlineStr">
         <is>
           <t>1.779,22</t>
         </is>
@@ -6266,6 +7354,17 @@
       </c>
       <c r="L103" t="inlineStr">
         <is>
+          <t>36:00</t>
+        </is>
+      </c>
+      <c r="M103" t="inlineStr"/>
+      <c r="N103" t="inlineStr">
+        <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="O103" t="inlineStr">
+        <is>
           <t>835,43</t>
         </is>
       </c>
@@ -6324,6 +7423,17 @@
       </c>
       <c r="L104" t="inlineStr">
         <is>
+          <t>9:00</t>
+        </is>
+      </c>
+      <c r="M104" t="inlineStr"/>
+      <c r="N104" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="O104" t="inlineStr">
+        <is>
           <t>1.074,92</t>
         </is>
       </c>
@@ -6382,6 +7492,17 @@
       </c>
       <c r="L105" t="inlineStr">
         <is>
+          <t>48:00</t>
+        </is>
+      </c>
+      <c r="M105" t="inlineStr"/>
+      <c r="N105" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="O105" t="inlineStr">
+        <is>
           <t>1.505,84</t>
         </is>
       </c>
@@ -6440,6 +7561,17 @@
       </c>
       <c r="L106" t="inlineStr">
         <is>
+          <t>5:00</t>
+        </is>
+      </c>
+      <c r="M106" t="inlineStr"/>
+      <c r="N106" t="inlineStr">
+        <is>
+          <t>5:00</t>
+        </is>
+      </c>
+      <c r="O106" t="inlineStr">
+        <is>
           <t>994,08</t>
         </is>
       </c>
@@ -6496,7 +7628,14 @@
           <t>118</t>
         </is>
       </c>
-      <c r="L107" t="inlineStr">
+      <c r="L107" t="inlineStr"/>
+      <c r="M107" t="inlineStr"/>
+      <c r="N107" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="O107" t="inlineStr">
         <is>
           <t>1.518,02</t>
         </is>
@@ -6554,7 +7693,14 @@
           <t>145</t>
         </is>
       </c>
-      <c r="L108" t="inlineStr">
+      <c r="L108" t="inlineStr"/>
+      <c r="M108" t="inlineStr"/>
+      <c r="N108" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="O108" t="inlineStr">
         <is>
           <t>1.691,29</t>
         </is>
@@ -6614,6 +7760,21 @@
       </c>
       <c r="L109" t="inlineStr">
         <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="M109" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="N109" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="O109" t="inlineStr">
+        <is>
           <t>758,06</t>
         </is>
       </c>
@@ -6672,6 +7833,17 @@
       </c>
       <c r="L110" t="inlineStr">
         <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="M110" t="inlineStr"/>
+      <c r="N110" t="inlineStr">
+        <is>
+          <t>3:00</t>
+        </is>
+      </c>
+      <c r="O110" t="inlineStr">
+        <is>
           <t>1.241,92</t>
         </is>
       </c>
@@ -6728,7 +7900,14 @@
           <t>80</t>
         </is>
       </c>
-      <c r="L111" t="inlineStr">
+      <c r="L111" t="inlineStr"/>
+      <c r="M111" t="inlineStr"/>
+      <c r="N111" t="inlineStr">
+        <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="O111" t="inlineStr">
         <is>
           <t>993,12</t>
         </is>
@@ -6788,6 +7967,17 @@
       </c>
       <c r="L112" t="inlineStr">
         <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="M112" t="inlineStr"/>
+      <c r="N112" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="O112" t="inlineStr">
+        <is>
           <t>1.493,99</t>
         </is>
       </c>
@@ -6846,6 +8036,17 @@
       </c>
       <c r="L113" t="inlineStr">
         <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="M113" t="inlineStr"/>
+      <c r="N113" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="O113" t="inlineStr">
+        <is>
           <t>1.540,76</t>
         </is>
       </c>
@@ -6902,7 +8103,14 @@
           <t>112</t>
         </is>
       </c>
-      <c r="L114" t="inlineStr">
+      <c r="L114" t="inlineStr"/>
+      <c r="M114" t="inlineStr"/>
+      <c r="N114" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="O114" t="inlineStr">
         <is>
           <t>1.465,94</t>
         </is>
@@ -6960,7 +8168,14 @@
           <t>43</t>
         </is>
       </c>
-      <c r="L115" t="inlineStr">
+      <c r="L115" t="inlineStr"/>
+      <c r="M115" t="inlineStr"/>
+      <c r="N115" t="inlineStr">
+        <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="O115" t="inlineStr">
         <is>
           <t>1.361,56</t>
         </is>
@@ -7020,6 +8235,17 @@
       </c>
       <c r="L116" t="inlineStr">
         <is>
+          <t>84:00</t>
+        </is>
+      </c>
+      <c r="M116" t="inlineStr"/>
+      <c r="N116" t="inlineStr">
+        <is>
+          <t>7:00</t>
+        </is>
+      </c>
+      <c r="O116" t="inlineStr">
+        <is>
           <t>827,50</t>
         </is>
       </c>
@@ -7076,7 +8302,14 @@
           <t>99</t>
         </is>
       </c>
-      <c r="L117" t="inlineStr">
+      <c r="L117" t="inlineStr"/>
+      <c r="M117" t="inlineStr"/>
+      <c r="N117" t="inlineStr">
+        <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="O117" t="inlineStr">
         <is>
           <t>1.231,75</t>
         </is>
@@ -7128,6 +8361,17 @@
       <c r="K118" t="inlineStr"/>
       <c r="L118" t="inlineStr">
         <is>
+          <t>80:00</t>
+        </is>
+      </c>
+      <c r="M118" t="inlineStr"/>
+      <c r="N118" t="inlineStr">
+        <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="O118" t="inlineStr">
+        <is>
           <t>45,67</t>
         </is>
       </c>
@@ -7186,6 +8430,21 @@
       </c>
       <c r="L119" t="inlineStr">
         <is>
+          <t>41:00</t>
+        </is>
+      </c>
+      <c r="M119" t="inlineStr">
+        <is>
+          <t>42:00</t>
+        </is>
+      </c>
+      <c r="N119" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="O119" t="inlineStr">
+        <is>
           <t>350,07</t>
         </is>
       </c>
@@ -7244,6 +8503,17 @@
       </c>
       <c r="L120" t="inlineStr">
         <is>
+          <t>60:00</t>
+        </is>
+      </c>
+      <c r="M120" t="inlineStr"/>
+      <c r="N120" t="inlineStr">
+        <is>
+          <t>5:00</t>
+        </is>
+      </c>
+      <c r="O120" t="inlineStr">
+        <is>
           <t>497,31</t>
         </is>
       </c>
@@ -7302,6 +8572,17 @@
       </c>
       <c r="L121" t="inlineStr">
         <is>
+          <t>25:00</t>
+        </is>
+      </c>
+      <c r="M121" t="inlineStr"/>
+      <c r="N121" t="inlineStr">
+        <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="O121" t="inlineStr">
+        <is>
           <t>645,66</t>
         </is>
       </c>
@@ -7359,6 +8640,21 @@
         </is>
       </c>
       <c r="L122" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="M122" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="N122" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="O122" t="inlineStr">
         <is>
           <t>1.510,61</t>
         </is>
@@ -7410,6 +8706,21 @@
       <c r="K123" t="inlineStr"/>
       <c r="L123" t="inlineStr">
         <is>
+          <t>60:00</t>
+        </is>
+      </c>
+      <c r="M123" t="inlineStr">
+        <is>
+          <t>60:00</t>
+        </is>
+      </c>
+      <c r="N123" t="inlineStr">
+        <is>
+          <t>6:00</t>
+        </is>
+      </c>
+      <c r="O123" t="inlineStr">
+        <is>
           <t>69,69</t>
         </is>
       </c>
@@ -7466,7 +8777,14 @@
           <t>124</t>
         </is>
       </c>
-      <c r="L124" t="inlineStr">
+      <c r="L124" t="inlineStr"/>
+      <c r="M124" t="inlineStr"/>
+      <c r="N124" t="inlineStr">
+        <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="O124" t="inlineStr">
         <is>
           <t>1.486,05</t>
         </is>
@@ -7524,7 +8842,18 @@
           <t>98</t>
         </is>
       </c>
-      <c r="L125" t="inlineStr">
+      <c r="L125" t="inlineStr"/>
+      <c r="M125" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="N125" t="inlineStr">
+        <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="O125" t="inlineStr">
         <is>
           <t>1.185,23</t>
         </is>
@@ -7576,6 +8905,13 @@
       <c r="K126" t="inlineStr"/>
       <c r="L126" t="inlineStr">
         <is>
+          <t>85:00</t>
+        </is>
+      </c>
+      <c r="M126" t="inlineStr"/>
+      <c r="N126" t="inlineStr"/>
+      <c r="O126" t="inlineStr">
+        <is>
           <t>0,00</t>
         </is>
       </c>
@@ -7634,6 +8970,17 @@
       </c>
       <c r="L127" t="inlineStr">
         <is>
+          <t>60:00</t>
+        </is>
+      </c>
+      <c r="M127" t="inlineStr"/>
+      <c r="N127" t="inlineStr">
+        <is>
+          <t>6:00</t>
+        </is>
+      </c>
+      <c r="O127" t="inlineStr">
+        <is>
           <t>804,73</t>
         </is>
       </c>
@@ -7692,6 +9039,17 @@
       </c>
       <c r="L128" t="inlineStr">
         <is>
+          <t>48:00</t>
+        </is>
+      </c>
+      <c r="M128" t="inlineStr"/>
+      <c r="N128" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="O128" t="inlineStr">
+        <is>
           <t>1.293,89</t>
         </is>
       </c>
@@ -7750,6 +9108,17 @@
       </c>
       <c r="L129" t="inlineStr">
         <is>
+          <t>40:00</t>
+        </is>
+      </c>
+      <c r="M129" t="inlineStr"/>
+      <c r="N129" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="O129" t="inlineStr">
+        <is>
           <t>1.372,80</t>
         </is>
       </c>
@@ -7808,6 +9177,17 @@
       </c>
       <c r="L130" t="inlineStr">
         <is>
+          <t>25:00</t>
+        </is>
+      </c>
+      <c r="M130" t="inlineStr"/>
+      <c r="N130" t="inlineStr">
+        <is>
+          <t>5:00</t>
+        </is>
+      </c>
+      <c r="O130" t="inlineStr">
+        <is>
           <t>948,11</t>
         </is>
       </c>
@@ -7864,7 +9244,14 @@
           <t>132</t>
         </is>
       </c>
-      <c r="L131" t="inlineStr">
+      <c r="L131" t="inlineStr"/>
+      <c r="M131" t="inlineStr"/>
+      <c r="N131" t="inlineStr">
+        <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="O131" t="inlineStr">
         <is>
           <t>1.541,06</t>
         </is>
@@ -7922,7 +9309,18 @@
           <t>96</t>
         </is>
       </c>
-      <c r="L132" t="inlineStr">
+      <c r="L132" t="inlineStr"/>
+      <c r="M132" t="inlineStr">
+        <is>
+          <t>38:00</t>
+        </is>
+      </c>
+      <c r="N132" t="inlineStr">
+        <is>
+          <t>3:00</t>
+        </is>
+      </c>
+      <c r="O132" t="inlineStr">
         <is>
           <t>1.178,76</t>
         </is>
@@ -7980,7 +9378,18 @@
           <t>52</t>
         </is>
       </c>
-      <c r="L133" t="inlineStr">
+      <c r="L133" t="inlineStr"/>
+      <c r="M133" t="inlineStr">
+        <is>
+          <t>3:00</t>
+        </is>
+      </c>
+      <c r="N133" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="O133" t="inlineStr">
         <is>
           <t>719,28</t>
         </is>
@@ -8038,7 +9447,14 @@
           <t>50</t>
         </is>
       </c>
-      <c r="L134" t="inlineStr">
+      <c r="L134" t="inlineStr"/>
+      <c r="M134" t="inlineStr"/>
+      <c r="N134" t="inlineStr">
+        <is>
+          <t>6:00</t>
+        </is>
+      </c>
+      <c r="O134" t="inlineStr">
         <is>
           <t>673,82</t>
         </is>
@@ -8097,6 +9513,17 @@
         </is>
       </c>
       <c r="L135" t="inlineStr">
+        <is>
+          <t>82:00</t>
+        </is>
+      </c>
+      <c r="M135" t="inlineStr"/>
+      <c r="N135" t="inlineStr">
+        <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="O135" t="inlineStr">
         <is>
           <t>573,22</t>
         </is>
@@ -8148,6 +9575,13 @@
       <c r="K136" t="inlineStr"/>
       <c r="L136" t="inlineStr">
         <is>
+          <t>52:00</t>
+        </is>
+      </c>
+      <c r="M136" t="inlineStr"/>
+      <c r="N136" t="inlineStr"/>
+      <c r="O136" t="inlineStr">
+        <is>
           <t>0,00</t>
         </is>
       </c>
@@ -8206,6 +9640,17 @@
       </c>
       <c r="L137" t="inlineStr">
         <is>
+          <t>74:00</t>
+        </is>
+      </c>
+      <c r="M137" t="inlineStr"/>
+      <c r="N137" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="O137" t="inlineStr">
+        <is>
           <t>1.036,57</t>
         </is>
       </c>
@@ -8263,6 +9708,17 @@
         </is>
       </c>
       <c r="L138" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="M138" t="inlineStr"/>
+      <c r="N138" t="inlineStr">
+        <is>
+          <t>7:00</t>
+        </is>
+      </c>
+      <c r="O138" t="inlineStr">
         <is>
           <t>682,44</t>
         </is>
@@ -8312,7 +9768,10 @@
       <c r="I139" t="inlineStr"/>
       <c r="J139" t="inlineStr"/>
       <c r="K139" t="inlineStr"/>
-      <c r="L139" t="inlineStr">
+      <c r="L139" t="inlineStr"/>
+      <c r="M139" t="inlineStr"/>
+      <c r="N139" t="inlineStr"/>
+      <c r="O139" t="inlineStr">
         <is>
           <t>0,00</t>
         </is>
@@ -8370,7 +9829,14 @@
           <t>115</t>
         </is>
       </c>
-      <c r="L140" t="inlineStr">
+      <c r="L140" t="inlineStr"/>
+      <c r="M140" t="inlineStr"/>
+      <c r="N140" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="O140" t="inlineStr">
         <is>
           <t>1.453,28</t>
         </is>
@@ -8430,6 +9896,17 @@
       </c>
       <c r="L141" t="inlineStr">
         <is>
+          <t>25:00</t>
+        </is>
+      </c>
+      <c r="M141" t="inlineStr"/>
+      <c r="N141" t="inlineStr">
+        <is>
+          <t>5:00</t>
+        </is>
+      </c>
+      <c r="O141" t="inlineStr">
+        <is>
           <t>924,59</t>
         </is>
       </c>
@@ -8486,7 +9963,18 @@
           <t>107</t>
         </is>
       </c>
-      <c r="L142" t="inlineStr">
+      <c r="L142" t="inlineStr"/>
+      <c r="M142" t="inlineStr">
+        <is>
+          <t>38:00</t>
+        </is>
+      </c>
+      <c r="N142" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="O142" t="inlineStr">
         <is>
           <t>1.504,09</t>
         </is>
@@ -8544,7 +10032,14 @@
           <t>94</t>
         </is>
       </c>
-      <c r="L143" t="inlineStr">
+      <c r="L143" t="inlineStr"/>
+      <c r="M143" t="inlineStr"/>
+      <c r="N143" t="inlineStr">
+        <is>
+          <t>7:00</t>
+        </is>
+      </c>
+      <c r="O143" t="inlineStr">
         <is>
           <t>1.161,37</t>
         </is>
@@ -8596,6 +10091,17 @@
       <c r="K144" t="inlineStr"/>
       <c r="L144" t="inlineStr">
         <is>
+          <t>154:00</t>
+        </is>
+      </c>
+      <c r="M144" t="inlineStr"/>
+      <c r="N144" t="inlineStr">
+        <is>
+          <t>6:00</t>
+        </is>
+      </c>
+      <c r="O144" t="inlineStr">
+        <is>
           <t>68,57</t>
         </is>
       </c>
@@ -8644,7 +10150,10 @@
       <c r="I145" t="inlineStr"/>
       <c r="J145" t="inlineStr"/>
       <c r="K145" t="inlineStr"/>
-      <c r="L145" t="inlineStr">
+      <c r="L145" t="inlineStr"/>
+      <c r="M145" t="inlineStr"/>
+      <c r="N145" t="inlineStr"/>
+      <c r="O145" t="inlineStr">
         <is>
           <t>0,00</t>
         </is>
@@ -8704,6 +10213,17 @@
       </c>
       <c r="L146" t="inlineStr">
         <is>
+          <t>6:00</t>
+        </is>
+      </c>
+      <c r="M146" t="inlineStr"/>
+      <c r="N146" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="O146" t="inlineStr">
+        <is>
           <t>1.607,26</t>
         </is>
       </c>
@@ -8762,6 +10282,17 @@
       </c>
       <c r="L147" t="inlineStr">
         <is>
+          <t>53:00</t>
+        </is>
+      </c>
+      <c r="M147" t="inlineStr"/>
+      <c r="N147" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="O147" t="inlineStr">
+        <is>
           <t>1.042,55</t>
         </is>
       </c>
@@ -8816,6 +10347,17 @@
       </c>
       <c r="L148" t="inlineStr">
         <is>
+          <t>26:00</t>
+        </is>
+      </c>
+      <c r="M148" t="inlineStr"/>
+      <c r="N148" t="inlineStr">
+        <is>
+          <t>3:00</t>
+        </is>
+      </c>
+      <c r="O148" t="inlineStr">
+        <is>
           <t>705,92</t>
         </is>
       </c>
@@ -8874,6 +10416,17 @@
       </c>
       <c r="L149" t="inlineStr">
         <is>
+          <t>54:00</t>
+        </is>
+      </c>
+      <c r="M149" t="inlineStr"/>
+      <c r="N149" t="inlineStr">
+        <is>
+          <t>6:00</t>
+        </is>
+      </c>
+      <c r="O149" t="inlineStr">
+        <is>
           <t>1.236,89</t>
         </is>
       </c>
@@ -8930,7 +10483,14 @@
           <t>136</t>
         </is>
       </c>
-      <c r="L150" t="inlineStr">
+      <c r="L150" t="inlineStr"/>
+      <c r="M150" t="inlineStr"/>
+      <c r="N150" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="O150" t="inlineStr">
         <is>
           <t>1.593,35</t>
         </is>
@@ -8982,6 +10542,13 @@
       <c r="K151" t="inlineStr"/>
       <c r="L151" t="inlineStr">
         <is>
+          <t>52:00</t>
+        </is>
+      </c>
+      <c r="M151" t="inlineStr"/>
+      <c r="N151" t="inlineStr"/>
+      <c r="O151" t="inlineStr">
+        <is>
           <t>0,00</t>
         </is>
       </c>
@@ -9038,7 +10605,14 @@
           <t>86</t>
         </is>
       </c>
-      <c r="L152" t="inlineStr">
+      <c r="L152" t="inlineStr"/>
+      <c r="M152" t="inlineStr"/>
+      <c r="N152" t="inlineStr">
+        <is>
+          <t>6:00</t>
+        </is>
+      </c>
+      <c r="O152" t="inlineStr">
         <is>
           <t>1.059,59</t>
         </is>
@@ -9098,6 +10672,17 @@
       </c>
       <c r="L153" t="inlineStr">
         <is>
+          <t>24:00</t>
+        </is>
+      </c>
+      <c r="M153" t="inlineStr"/>
+      <c r="N153" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="O153" t="inlineStr">
+        <is>
           <t>1.020,20</t>
         </is>
       </c>
@@ -9155,6 +10740,17 @@
         </is>
       </c>
       <c r="L154" t="inlineStr">
+        <is>
+          <t>96:00</t>
+        </is>
+      </c>
+      <c r="M154" t="inlineStr"/>
+      <c r="N154" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="O154" t="inlineStr">
         <is>
           <t>357,29</t>
         </is>
@@ -9206,6 +10802,21 @@
       <c r="K155" t="inlineStr"/>
       <c r="L155" t="inlineStr">
         <is>
+          <t>76:00</t>
+        </is>
+      </c>
+      <c r="M155" t="inlineStr">
+        <is>
+          <t>68:00</t>
+        </is>
+      </c>
+      <c r="N155" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="O155" t="inlineStr">
+        <is>
           <t>91,69</t>
         </is>
       </c>
@@ -9262,7 +10873,14 @@
           <t>144</t>
         </is>
       </c>
-      <c r="L156" t="inlineStr">
+      <c r="L156" t="inlineStr"/>
+      <c r="M156" t="inlineStr"/>
+      <c r="N156" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="O156" t="inlineStr">
         <is>
           <t>1.667,41</t>
         </is>
@@ -9320,7 +10938,14 @@
           <t>115</t>
         </is>
       </c>
-      <c r="L157" t="inlineStr">
+      <c r="L157" t="inlineStr"/>
+      <c r="M157" t="inlineStr"/>
+      <c r="N157" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="O157" t="inlineStr">
         <is>
           <t>1.515,71</t>
         </is>
@@ -9378,7 +11003,14 @@
           <t>145</t>
         </is>
       </c>
-      <c r="L158" t="inlineStr">
+      <c r="L158" t="inlineStr"/>
+      <c r="M158" t="inlineStr"/>
+      <c r="N158" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="O158" t="inlineStr">
         <is>
           <t>1.766,57</t>
         </is>
@@ -9436,7 +11068,14 @@
           <t>152</t>
         </is>
       </c>
-      <c r="L159" t="inlineStr">
+      <c r="L159" t="inlineStr"/>
+      <c r="M159" t="inlineStr"/>
+      <c r="N159" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="O159" t="inlineStr">
         <is>
           <t>1.687,55</t>
         </is>
@@ -9494,7 +11133,14 @@
           <t>127</t>
         </is>
       </c>
-      <c r="L160" t="inlineStr">
+      <c r="L160" t="inlineStr"/>
+      <c r="M160" t="inlineStr"/>
+      <c r="N160" t="inlineStr">
+        <is>
+          <t>6:00</t>
+        </is>
+      </c>
+      <c r="O160" t="inlineStr">
         <is>
           <t>1.674,72</t>
         </is>
@@ -9554,6 +11200,17 @@
       </c>
       <c r="L161" t="inlineStr">
         <is>
+          <t>74:00</t>
+        </is>
+      </c>
+      <c r="M161" t="inlineStr"/>
+      <c r="N161" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="O161" t="inlineStr">
+        <is>
           <t>886,51</t>
         </is>
       </c>
@@ -9612,6 +11269,17 @@
       </c>
       <c r="L162" t="inlineStr">
         <is>
+          <t>42:00</t>
+        </is>
+      </c>
+      <c r="M162" t="inlineStr"/>
+      <c r="N162" t="inlineStr">
+        <is>
+          <t>5:00</t>
+        </is>
+      </c>
+      <c r="O162" t="inlineStr">
+        <is>
           <t>840,15</t>
         </is>
       </c>
@@ -9670,6 +11338,17 @@
       </c>
       <c r="L163" t="inlineStr">
         <is>
+          <t>7:00</t>
+        </is>
+      </c>
+      <c r="M163" t="inlineStr"/>
+      <c r="N163" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="O163" t="inlineStr">
+        <is>
           <t>1.350,91</t>
         </is>
       </c>
@@ -9728,6 +11407,17 @@
       </c>
       <c r="L164" t="inlineStr">
         <is>
+          <t>61:00</t>
+        </is>
+      </c>
+      <c r="M164" t="inlineStr"/>
+      <c r="N164" t="inlineStr">
+        <is>
+          <t>5:00</t>
+        </is>
+      </c>
+      <c r="O164" t="inlineStr">
+        <is>
           <t>1.075,40</t>
         </is>
       </c>
@@ -9786,6 +11476,21 @@
       </c>
       <c r="L165" t="inlineStr">
         <is>
+          <t>38:00</t>
+        </is>
+      </c>
+      <c r="M165" t="inlineStr">
+        <is>
+          <t>68:00</t>
+        </is>
+      </c>
+      <c r="N165" t="inlineStr">
+        <is>
+          <t>7:00</t>
+        </is>
+      </c>
+      <c r="O165" t="inlineStr">
+        <is>
           <t>795,12</t>
         </is>
       </c>
@@ -9842,7 +11547,18 @@
           <t>115</t>
         </is>
       </c>
-      <c r="L166" t="inlineStr">
+      <c r="L166" t="inlineStr"/>
+      <c r="M166" t="inlineStr">
+        <is>
+          <t>29:00</t>
+        </is>
+      </c>
+      <c r="N166" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="O166" t="inlineStr">
         <is>
           <t>1.845,60</t>
         </is>
@@ -9902,6 +11618,17 @@
       </c>
       <c r="L167" t="inlineStr">
         <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="M167" t="inlineStr"/>
+      <c r="N167" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="O167" t="inlineStr">
+        <is>
           <t>1.738,79</t>
         </is>
       </c>
@@ -9958,7 +11685,18 @@
           <t>122</t>
         </is>
       </c>
-      <c r="L168" t="inlineStr">
+      <c r="L168" t="inlineStr"/>
+      <c r="M168" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="N168" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="O168" t="inlineStr">
         <is>
           <t>1.592,19</t>
         </is>
@@ -10016,7 +11754,14 @@
           <t>51</t>
         </is>
       </c>
-      <c r="L169" t="inlineStr">
+      <c r="L169" t="inlineStr"/>
+      <c r="M169" t="inlineStr"/>
+      <c r="N169" t="inlineStr">
+        <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="O169" t="inlineStr">
         <is>
           <t>659,35</t>
         </is>
@@ -10074,7 +11819,14 @@
           <t>78</t>
         </is>
       </c>
-      <c r="L170" t="inlineStr">
+      <c r="L170" t="inlineStr"/>
+      <c r="M170" t="inlineStr"/>
+      <c r="N170" t="inlineStr">
+        <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="O170" t="inlineStr">
         <is>
           <t>1.241,56</t>
         </is>
@@ -10132,7 +11884,14 @@
           <t>15</t>
         </is>
       </c>
-      <c r="L171" t="inlineStr">
+      <c r="L171" t="inlineStr"/>
+      <c r="M171" t="inlineStr"/>
+      <c r="N171" t="inlineStr">
+        <is>
+          <t>3:00</t>
+        </is>
+      </c>
+      <c r="O171" t="inlineStr">
         <is>
           <t>491,39</t>
         </is>
@@ -10192,6 +11951,17 @@
       </c>
       <c r="L172" t="inlineStr">
         <is>
+          <t>6:00</t>
+        </is>
+      </c>
+      <c r="M172" t="inlineStr"/>
+      <c r="N172" t="inlineStr">
+        <is>
+          <t>3:00</t>
+        </is>
+      </c>
+      <c r="O172" t="inlineStr">
+        <is>
           <t>673,99</t>
         </is>
       </c>
@@ -10248,7 +12018,14 @@
           <t>140</t>
         </is>
       </c>
-      <c r="L173" t="inlineStr">
+      <c r="L173" t="inlineStr"/>
+      <c r="M173" t="inlineStr"/>
+      <c r="N173" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="O173" t="inlineStr">
         <is>
           <t>1.644,40</t>
         </is>
@@ -10306,7 +12083,14 @@
           <t>124</t>
         </is>
       </c>
-      <c r="L174" t="inlineStr">
+      <c r="L174" t="inlineStr"/>
+      <c r="M174" t="inlineStr"/>
+      <c r="N174" t="inlineStr">
+        <is>
+          <t>3:00</t>
+        </is>
+      </c>
+      <c r="O174" t="inlineStr">
         <is>
           <t>1.424,06</t>
         </is>
@@ -10364,7 +12148,14 @@
           <t>74</t>
         </is>
       </c>
-      <c r="L175" t="inlineStr">
+      <c r="L175" t="inlineStr"/>
+      <c r="M175" t="inlineStr"/>
+      <c r="N175" t="inlineStr">
+        <is>
+          <t>3:00</t>
+        </is>
+      </c>
+      <c r="O175" t="inlineStr">
         <is>
           <t>893,75</t>
         </is>
@@ -10422,7 +12213,14 @@
           <t>89</t>
         </is>
       </c>
-      <c r="L176" t="inlineStr">
+      <c r="L176" t="inlineStr"/>
+      <c r="M176" t="inlineStr"/>
+      <c r="N176" t="inlineStr">
+        <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="O176" t="inlineStr">
         <is>
           <t>1.066,87</t>
         </is>
@@ -10480,7 +12278,14 @@
           <t>109</t>
         </is>
       </c>
-      <c r="L177" t="inlineStr">
+      <c r="L177" t="inlineStr"/>
+      <c r="M177" t="inlineStr"/>
+      <c r="N177" t="inlineStr">
+        <is>
+          <t>5:00</t>
+        </is>
+      </c>
+      <c r="O177" t="inlineStr">
         <is>
           <t>1.344,41</t>
         </is>
@@ -10538,13 +12343,22 @@
           <t>89</t>
         </is>
       </c>
-      <c r="L178" t="inlineStr">
+      <c r="L178" t="inlineStr"/>
+      <c r="M178" t="inlineStr"/>
+      <c r="N178" t="inlineStr">
+        <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="O178" t="inlineStr">
         <is>
           <t>1.095,36</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>